<commit_message>
"fixed: outputting specials and exclusive"
</commit_message>
<xml_diff>
--- a/Week-2/FoodMenu/Menu.xlsx
+++ b/Week-2/FoodMenu/Menu.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <x:si>
     <x:t>DishName</x:t>
   </x:si>
@@ -68,6 +68,12 @@
   </x:si>
   <x:si>
     <x:t>FISH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>blueberry</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ice cream</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -578,6 +584,34 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="A13" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="n">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4">
+      <x:c r="A14" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="n">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="b">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="b">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>